<commit_message>
add nb changes to AA count
</commit_message>
<xml_diff>
--- a/analyses/05.22.17-55m-2500m-AAtots.xlsx
+++ b/analyses/05.22.17-55m-2500m-AAtots.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="13660"/>
+    <workbookView xWindow="1440" yWindow="460" windowWidth="24640" windowHeight="13660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="05.22.17_55m_db_tryp" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2480" uniqueCount="1188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="1211">
   <si>
     <t>Peptide</t>
   </si>
@@ -3583,13 +3584,82 @@
   </si>
   <si>
     <t>CTNVTKGGK</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Amino acid</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>depth (m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3720,6 +3790,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4066,9 +4144,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4426,8 +4506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P790"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4435,6 +4515,7 @@
     <col min="1" max="1" width="27.83203125" customWidth="1"/>
     <col min="13" max="13" width="157.5" customWidth="1"/>
     <col min="14" max="14" width="43.1640625" customWidth="1"/>
+    <col min="15" max="15" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -38966,4 +39047,1024 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B1">
+        <v>97</v>
+      </c>
+      <c r="C1">
+        <v>97</v>
+      </c>
+      <c r="D1">
+        <v>111</v>
+      </c>
+      <c r="E1">
+        <v>111</v>
+      </c>
+      <c r="F1">
+        <v>264</v>
+      </c>
+      <c r="G1">
+        <v>264</v>
+      </c>
+      <c r="H1">
+        <v>265</v>
+      </c>
+      <c r="J1">
+        <v>266</v>
+      </c>
+      <c r="L1">
+        <v>267</v>
+      </c>
+      <c r="M1">
+        <v>268</v>
+      </c>
+      <c r="N1">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B2" s="2">
+        <v>710</v>
+      </c>
+      <c r="D2" s="2">
+        <v>105</v>
+      </c>
+      <c r="F2" s="2">
+        <v>94</v>
+      </c>
+      <c r="H2" s="2">
+        <v>94</v>
+      </c>
+      <c r="J2" s="2">
+        <v>265</v>
+      </c>
+      <c r="L2" s="2">
+        <v>265</v>
+      </c>
+      <c r="M2" s="2">
+        <v>965</v>
+      </c>
+      <c r="N2" s="2">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B3">
+        <v>721</v>
+      </c>
+      <c r="C3">
+        <f>B3/$B$23</f>
+        <v>8.7638264251853656E-2</v>
+      </c>
+      <c r="D3">
+        <v>1046</v>
+      </c>
+      <c r="E3">
+        <f>D3/$D$23</f>
+        <v>8.8599017448754869E-2</v>
+      </c>
+      <c r="F3">
+        <v>711</v>
+      </c>
+      <c r="G3">
+        <f>F3/$F$23</f>
+        <v>7.7391966909763799E-2</v>
+      </c>
+      <c r="H3">
+        <v>651</v>
+      </c>
+      <c r="I3">
+        <f>H3/$H$23</f>
+        <v>7.3926868044515107E-2</v>
+      </c>
+      <c r="J3">
+        <v>124</v>
+      </c>
+      <c r="L3">
+        <v>131</v>
+      </c>
+      <c r="M3">
+        <v>1132</v>
+      </c>
+      <c r="N3">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B4">
+        <v>653</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C22" si="0">B4/$B$23</f>
+        <v>7.9372796888294642E-2</v>
+      </c>
+      <c r="D4">
+        <v>672</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E22" si="1">D4/$D$23</f>
+        <v>5.6920210062679992E-2</v>
+      </c>
+      <c r="F4">
+        <v>460</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G22" si="2">F4/$F$23</f>
+        <v>5.0070752149776861E-2</v>
+      </c>
+      <c r="H4">
+        <v>520</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I22" si="3">H4/$H$23</f>
+        <v>5.90506472859414E-2</v>
+      </c>
+      <c r="J4">
+        <v>97</v>
+      </c>
+      <c r="L4">
+        <v>137</v>
+      </c>
+      <c r="M4">
+        <v>684</v>
+      </c>
+      <c r="N4">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B5">
+        <v>422</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5.1294518050322112E-2</v>
+      </c>
+      <c r="D5">
+        <v>509</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>4.3113671014738265E-2</v>
+      </c>
+      <c r="F5">
+        <v>409</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>4.451942962882334E-2</v>
+      </c>
+      <c r="H5">
+        <v>369</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>4.1903247785600728E-2</v>
+      </c>
+      <c r="J5">
+        <v>69</v>
+      </c>
+      <c r="L5">
+        <v>102</v>
+      </c>
+      <c r="M5">
+        <v>857</v>
+      </c>
+      <c r="N5">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B6">
+        <v>372</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>4.5216968518293425E-2</v>
+      </c>
+      <c r="D6">
+        <v>777</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>6.5813992884973749E-2</v>
+      </c>
+      <c r="F6">
+        <v>475</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>5.1703494067704366E-2</v>
+      </c>
+      <c r="H6">
+        <v>493</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>5.5984555984555984E-2</v>
+      </c>
+      <c r="J6">
+        <v>87</v>
+      </c>
+      <c r="L6">
+        <v>106</v>
+      </c>
+      <c r="M6">
+        <v>1136</v>
+      </c>
+      <c r="N6">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B7">
+        <v>175</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>2.1271423362100399E-2</v>
+      </c>
+      <c r="D7">
+        <v>172</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1.4568863289852617E-2</v>
+      </c>
+      <c r="F7">
+        <v>159</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>1.7307064330031565E-2</v>
+      </c>
+      <c r="H7">
+        <v>120</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>1.3627072450601862E-2</v>
+      </c>
+      <c r="J7">
+        <v>29</v>
+      </c>
+      <c r="L7">
+        <v>62</v>
+      </c>
+      <c r="M7">
+        <v>239</v>
+      </c>
+      <c r="N7">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B8">
+        <v>326</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>3.962562294882703E-2</v>
+      </c>
+      <c r="D8">
+        <v>449</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>3.8031509401998981E-2</v>
+      </c>
+      <c r="F8">
+        <v>323</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>3.515837596603897E-2</v>
+      </c>
+      <c r="H8">
+        <v>279</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>3.1682943447649332E-2</v>
+      </c>
+      <c r="J8">
+        <v>49</v>
+      </c>
+      <c r="L8">
+        <v>75</v>
+      </c>
+      <c r="M8">
+        <v>469</v>
+      </c>
+      <c r="N8">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B9">
+        <v>428</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>5.2023823994165552E-2</v>
+      </c>
+      <c r="D9">
+        <v>1240</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0.10503133999661189</v>
+      </c>
+      <c r="F9">
+        <v>565</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>6.1499945575269402E-2</v>
+      </c>
+      <c r="H9">
+        <v>678</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>7.6992959345900516E-2</v>
+      </c>
+      <c r="J9">
+        <v>77</v>
+      </c>
+      <c r="L9">
+        <v>132</v>
+      </c>
+      <c r="M9">
+        <v>1613</v>
+      </c>
+      <c r="N9">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B10">
+        <v>429</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>5.2145374984806127E-2</v>
+      </c>
+      <c r="D10">
+        <v>398</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>3.3711672031170592E-2</v>
+      </c>
+      <c r="F10">
+        <v>292</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>3.1784042668988786E-2</v>
+      </c>
+      <c r="H10">
+        <v>319</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>3.6225300931183285E-2</v>
+      </c>
+      <c r="J10">
+        <v>61</v>
+      </c>
+      <c r="L10">
+        <v>94</v>
+      </c>
+      <c r="M10">
+        <v>527</v>
+      </c>
+      <c r="N10">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B11">
+        <v>144</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1.7503342652242616E-2</v>
+      </c>
+      <c r="D11">
+        <v>130</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>1.1011350160935117E-2</v>
+      </c>
+      <c r="F11">
+        <v>301</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>3.2763687819745292E-2</v>
+      </c>
+      <c r="H11">
+        <v>264</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>2.9979559391324098E-2</v>
+      </c>
+      <c r="J11">
+        <v>46</v>
+      </c>
+      <c r="L11">
+        <v>56</v>
+      </c>
+      <c r="M11">
+        <v>441</v>
+      </c>
+      <c r="N11">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B13">
+        <v>931</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.11316397228637413</v>
+      </c>
+      <c r="D13">
+        <v>2052</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0.17380992715568355</v>
+      </c>
+      <c r="F13">
+        <v>782</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>8.5120278654620657E-2</v>
+      </c>
+      <c r="H13">
+        <v>750</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>8.5169202816261641E-2</v>
+      </c>
+      <c r="J13">
+        <v>150</v>
+      </c>
+      <c r="L13">
+        <v>188</v>
+      </c>
+      <c r="M13">
+        <v>1944</v>
+      </c>
+      <c r="N13">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B14">
+        <v>594</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>7.2201288440500791E-2</v>
+      </c>
+      <c r="D14">
+        <v>872</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>7.3860748771810938E-2</v>
+      </c>
+      <c r="F14">
+        <v>1119</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>0.12180254707739196</v>
+      </c>
+      <c r="H14">
+        <v>1023</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>0.11617079264138087</v>
+      </c>
+      <c r="J14">
+        <v>139</v>
+      </c>
+      <c r="L14">
+        <v>172</v>
+      </c>
+      <c r="M14">
+        <v>2184</v>
+      </c>
+      <c r="N14">
+        <v>3318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B15">
+        <v>328</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>3.9868724930108179E-2</v>
+      </c>
+      <c r="D15">
+        <v>304</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>2.5749618837879046E-2</v>
+      </c>
+      <c r="F15">
+        <v>603</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>6.5636225100685758E-2</v>
+      </c>
+      <c r="H15">
+        <v>490</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>5.5643879173290937E-2</v>
+      </c>
+      <c r="J15">
+        <v>65</v>
+      </c>
+      <c r="L15">
+        <v>96</v>
+      </c>
+      <c r="M15">
+        <v>1053</v>
+      </c>
+      <c r="N15">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B16">
+        <v>293</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>3.5614440257688097E-2</v>
+      </c>
+      <c r="D16">
+        <v>527</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>4.4638319498560057E-2</v>
+      </c>
+      <c r="F16">
+        <v>341</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>3.7117666267551974E-2</v>
+      </c>
+      <c r="H16">
+        <v>272</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>3.0888030888030889E-2</v>
+      </c>
+      <c r="J16">
+        <v>59</v>
+      </c>
+      <c r="L16">
+        <v>65</v>
+      </c>
+      <c r="M16">
+        <v>684</v>
+      </c>
+      <c r="N16">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B17">
+        <v>424</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>5.1537620031603261E-2</v>
+      </c>
+      <c r="D17">
+        <v>228</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1.9312214128409284E-2</v>
+      </c>
+      <c r="F17">
+        <v>541</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>5.8887558506585391E-2</v>
+      </c>
+      <c r="H17">
+        <v>555</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>6.3025210084033612E-2</v>
+      </c>
+      <c r="J17">
+        <v>95</v>
+      </c>
+      <c r="L17">
+        <v>121</v>
+      </c>
+      <c r="M17">
+        <v>1112</v>
+      </c>
+      <c r="N17">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B18">
+        <v>483</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>5.8709128479397105E-2</v>
+      </c>
+      <c r="D18">
+        <v>561</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>4.7518211079112319E-2</v>
+      </c>
+      <c r="F18">
+        <v>401</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>4.3648633939262001E-2</v>
+      </c>
+      <c r="H18">
+        <v>428</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>4.860322507381331E-2</v>
+      </c>
+      <c r="J18">
+        <v>78</v>
+      </c>
+      <c r="L18">
+        <v>97</v>
+      </c>
+      <c r="M18">
+        <v>652</v>
+      </c>
+      <c r="N18">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B19">
+        <v>470</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>5.7128965601069649E-2</v>
+      </c>
+      <c r="D19">
+        <v>626</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>5.3023886159579876E-2</v>
+      </c>
+      <c r="F19">
+        <v>572</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>6.2261891803635575E-2</v>
+      </c>
+      <c r="H19">
+        <v>511</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>5.8028616852146261E-2</v>
+      </c>
+      <c r="J19">
+        <v>79</v>
+      </c>
+      <c r="L19">
+        <v>97</v>
+      </c>
+      <c r="M19">
+        <v>924</v>
+      </c>
+      <c r="N19">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B20">
+        <v>161</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1.9569709493132369E-2</v>
+      </c>
+      <c r="D20">
+        <v>112</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>9.4867016771133326E-3</v>
+      </c>
+      <c r="F20">
+        <v>237</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>2.57973223032546E-2</v>
+      </c>
+      <c r="H20">
+        <v>206</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>2.3393141040199864E-2</v>
+      </c>
+      <c r="J20">
+        <v>40</v>
+      </c>
+      <c r="L20">
+        <v>54</v>
+      </c>
+      <c r="M20">
+        <v>381</v>
+      </c>
+      <c r="N20">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B21">
+        <v>295</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>3.5857542238969246E-2</v>
+      </c>
+      <c r="D21">
+        <v>392</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>3.3203455869896661E-2</v>
+      </c>
+      <c r="F21">
+        <v>301</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>3.2763687819745292E-2</v>
+      </c>
+      <c r="H21">
+        <v>272</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>3.0888030888030889E-2</v>
+      </c>
+      <c r="J21">
+        <v>42</v>
+      </c>
+      <c r="L21">
+        <v>67</v>
+      </c>
+      <c r="M21">
+        <v>341</v>
+      </c>
+      <c r="N21">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B22">
+        <v>578</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>7.0256472590251612E-2</v>
+      </c>
+      <c r="D22">
+        <v>739</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>6.2595290530238865E-2</v>
+      </c>
+      <c r="F22">
+        <v>595</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>6.4765429411124412E-2</v>
+      </c>
+      <c r="H22">
+        <v>606</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>6.8816715875539405E-2</v>
+      </c>
+      <c r="J22">
+        <v>123</v>
+      </c>
+      <c r="L22">
+        <v>159</v>
+      </c>
+      <c r="M22">
+        <v>1256</v>
+      </c>
+      <c r="N22">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="3" customFormat="1">
+      <c r="A23" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B23" s="3">
+        <f>SUM(B3:B22)</f>
+        <v>8227</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" ref="D23:N23" si="4">SUM(D3:D22)</f>
+        <v>11806</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="4"/>
+        <v>9187</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="4"/>
+        <v>8806</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="4"/>
+        <v>1509</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="4"/>
+        <v>2011</v>
+      </c>
+      <c r="M23" s="3">
+        <f t="shared" si="4"/>
+        <v>17629</v>
+      </c>
+      <c r="N23" s="3">
+        <f t="shared" si="4"/>
+        <v>27528</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>